<commit_message>
gets graph working, changed data to display only top 5 movies per day, adds color
</commit_message>
<xml_diff>
--- a/public/data/June Movie Data.xlsx
+++ b/public/data/June Movie Data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="826" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="826" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="354">
   <si>
     <t>Movie</t>
   </si>
@@ -1073,15 +1074,25 @@
   </si>
   <si>
     <t>GrossSales</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1163,7 +1174,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1183,8 +1194,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1200,8 +1213,10 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1219,6 +1234,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -13985,8 +14002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C92" sqref="B92:C101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="A1:C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17672,4 +17689,1837 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C151"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="15">
+        <v>41791</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="14">
+        <v>19383198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="15">
+        <v>41791</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="14">
+        <v>9339859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="15">
+        <v>41791</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="14">
+        <v>4231615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="15">
+        <v>41791</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3417587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="15">
+        <v>41791</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2129605</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="15">
+        <v>41792</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="14">
+        <v>6207742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="15">
+        <v>41792</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14">
+        <v>3163908</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="15">
+        <v>41792</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1627855</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="15">
+        <v>41792</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1152979</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="15">
+        <v>41792</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="14">
+        <v>911525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="15">
+        <v>41793</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="14">
+        <v>7196208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="15">
+        <v>41793</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="14">
+        <v>3787895</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="15">
+        <v>41793</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1864635</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="15">
+        <v>41793</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1370135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="15">
+        <v>41793</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="14">
+        <v>1059450</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="15">
+        <v>41794</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="14">
+        <v>5612603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="15">
+        <v>41794</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="14">
+        <v>2824137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="15">
+        <v>41794</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1419590</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="15">
+        <v>41794</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1117001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="15">
+        <v>41794</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="14">
+        <v>897550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="15">
+        <v>41795</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="14">
+        <v>5399117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="15">
+        <v>41795</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2605125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="15">
+        <v>41795</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1280505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="15">
+        <v>41795</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1013205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="15">
+        <v>41795</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="14">
+        <v>765605</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="15">
+        <v>41796</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="14">
+        <v>26062046</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="15">
+        <v>41796</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="14">
+        <v>10605165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="15">
+        <v>41796</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="14">
+        <v>10189870</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="15">
+        <v>41796</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="14">
+        <v>4510017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="15">
+        <v>41796</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2260790</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="15">
+        <v>41797</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="14">
+        <v>13463278</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="15">
+        <v>41797</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="14">
+        <v>12680655</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="15">
+        <v>41797</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="14">
+        <v>10474234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="15">
+        <v>41797</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="14">
+        <v>6176540</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="15">
+        <v>41797</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="14">
+        <v>2908685</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="15">
+        <v>41798</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="14">
+        <v>10675116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="15">
+        <v>41798</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="14">
+        <v>9259822</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="15">
+        <v>41798</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="14">
+        <v>7680847</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="15">
+        <v>41798</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="14">
+        <v>4468257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="15">
+        <v>41798</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="14">
+        <v>2179020</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="15">
+        <v>41799</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="14">
+        <v>5095488</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="15">
+        <v>41799</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="14">
+        <v>4047865</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="15">
+        <v>41799</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="14">
+        <v>3167460</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="15">
+        <v>41799</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="14">
+        <v>1765307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="15">
+        <v>41799</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="14">
+        <v>917935</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="15">
+        <v>41800</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="14">
+        <v>5002851</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="15">
+        <v>41800</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="14">
+        <v>4712585</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="15">
+        <v>41800</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="14">
+        <v>3482263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="15">
+        <v>41800</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="14">
+        <v>2021629</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="15">
+        <v>41800</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="14">
+        <v>1058440</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="15">
+        <v>41801</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="14">
+        <v>4168922</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="15">
+        <v>41801</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="14">
+        <v>3986901</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="15">
+        <v>41801</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="14">
+        <v>2772354</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="15">
+        <v>41801</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="14">
+        <v>1707464</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="15">
+        <v>41801</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="14">
+        <v>914865</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="15">
+        <v>41802</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="14">
+        <v>3705483</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="15">
+        <v>41802</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="14">
+        <v>3593949</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="15">
+        <v>41802</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="14">
+        <v>2292160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="15">
+        <v>41802</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="14">
+        <v>1389681</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="15">
+        <v>41802</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="14">
+        <v>630915</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="15">
+        <v>41803</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="14">
+        <v>25144490</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="15">
+        <v>41803</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="14">
+        <v>18440040</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="15">
+        <v>41803</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="14">
+        <v>6359826</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="15">
+        <v>41803</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="14">
+        <v>5848429</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="15">
+        <v>41803</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" s="14">
+        <v>4581413</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="15">
+        <v>41804</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="14">
+        <v>18726869</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="15">
+        <v>41804</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="14">
+        <v>17315466</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="15">
+        <v>41804</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" s="14">
+        <v>7311521</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="15">
+        <v>41804</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" s="14">
+        <v>6108727</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="15">
+        <v>41804</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="14">
+        <v>5741160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="15">
+        <v>41805</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="14">
+        <v>13695816</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="15">
+        <v>41805</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="14">
+        <v>13200086</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="15">
+        <v>41805</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" s="14">
+        <v>5837075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="15">
+        <v>41805</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="14">
+        <v>5345047</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="15">
+        <v>41805</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="14">
+        <v>3360831</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="15">
+        <v>41806</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="14">
+        <v>6830926</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="15">
+        <v>41806</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="14">
+        <v>5056288</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="15">
+        <v>41806</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="14">
+        <v>2307777</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="15">
+        <v>41806</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" s="14">
+        <v>2269929</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="15">
+        <v>41806</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="14">
+        <v>1672018</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="15">
+        <v>41807</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="14">
+        <v>7348908</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="15">
+        <v>41807</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="14">
+        <v>5905504</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="15">
+        <v>41807</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" s="14">
+        <v>2841610</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="15">
+        <v>41807</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="14">
+        <v>2641279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="15">
+        <v>41807</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="14">
+        <v>2083413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="15">
+        <v>41808</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" s="14">
+        <v>5774371</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="15">
+        <v>41808</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="14">
+        <v>4778724</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="15">
+        <v>41808</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="14">
+        <v>2393514</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="15">
+        <v>41808</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" s="14">
+        <v>2233298</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="15">
+        <v>41808</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" s="14">
+        <v>1711035</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="15">
+        <v>41809</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="14">
+        <v>5424480</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="15">
+        <v>41809</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="14">
+        <v>4684897</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="15">
+        <v>41809</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="14">
+        <v>2441986</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="15">
+        <v>41809</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" s="14">
+        <v>2178779</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="15">
+        <v>41809</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" s="14">
+        <v>1703329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="15">
+        <v>41810</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C97" s="14">
+        <v>12180056</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="15">
+        <v>41810</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="14">
+        <v>9325176</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="15">
+        <v>41810</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="14">
+        <v>7636170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="15">
+        <v>41810</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="14">
+        <v>4644888</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="15">
+        <v>41810</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C101" s="14">
+        <v>3999121</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="15">
+        <v>41811</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="14">
+        <v>10812737</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="15">
+        <v>41811</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C103" s="14">
+        <v>10308403</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="15">
+        <v>41811</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="14">
+        <v>10066297</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="15">
+        <v>41811</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C105" s="14">
+        <v>5250652</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="15">
+        <v>41811</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C106" s="14">
+        <v>5215367</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="15">
+        <v>41812</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="14">
+        <v>7323082</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="15">
+        <v>41812</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="14">
+        <v>7016845</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="15">
+        <v>41812</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="14">
+        <v>6753452</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="15">
+        <v>41812</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C110" s="14">
+        <v>3660993</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="15">
+        <v>41812</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C111" s="14">
+        <v>3459116</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="15">
+        <v>41813</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="14">
+        <v>3638450</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="15">
+        <v>41813</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" s="14">
+        <v>3123254</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="15">
+        <v>41813</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" s="14">
+        <v>2475300</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="15">
+        <v>41813</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C115" s="14">
+        <v>1748844</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="15">
+        <v>41813</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" s="14">
+        <v>1472498</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="15">
+        <v>41814</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="14">
+        <v>4465576</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="15">
+        <v>41814</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" s="14">
+        <v>4336155</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="15">
+        <v>41814</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119" s="14">
+        <v>2559902</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="15">
+        <v>41814</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C120" s="14">
+        <v>2315415</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="15">
+        <v>41814</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C121" s="14">
+        <v>1933409</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="15">
+        <v>41815</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" s="14">
+        <v>3524302</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="15">
+        <v>41815</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C123" s="14">
+        <v>3492276</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="15">
+        <v>41815</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C124" s="14">
+        <v>1941335</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="15">
+        <v>41815</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C125" s="14">
+        <v>1862648</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="15">
+        <v>41815</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C126" s="14">
+        <v>1604028</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="15">
+        <v>41816</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C127" s="14">
+        <v>2929465</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="15">
+        <v>41816</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C128" s="14">
+        <v>1748462</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="15">
+        <v>41816</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" s="14">
+        <v>1628599</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="15">
+        <v>41816</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C130" s="14">
+        <v>1403180</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="15">
+        <v>41816</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="14">
+        <v>1352963</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="15">
+        <v>41817</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C132" s="14">
+        <v>5135431</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="15">
+        <v>41817</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C133" s="14">
+        <v>4120789</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="15">
+        <v>41817</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="14">
+        <v>3383399</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="15">
+        <v>41817</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" s="14">
+        <v>2598651</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="15">
+        <v>41817</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C136" s="14">
+        <v>2259438</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="15">
+        <v>41818</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" s="14">
+        <v>6172211</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="15">
+        <v>41818</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C138" s="14">
+        <v>5156662</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="15">
+        <v>41818</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" s="14">
+        <v>4258372</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="15">
+        <v>41818</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C140" s="14">
+        <v>3307493</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="15">
+        <v>41818</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" s="14">
+        <v>3163706</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="16">
+        <v>41819</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" s="14">
+        <v>4534733</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="16">
+        <v>41819</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" s="14">
+        <v>3960246</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="16">
+        <v>41819</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144" s="14">
+        <v>2674626</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="16">
+        <v>41819</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C145" s="14">
+        <v>2470530</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="16">
+        <v>41819</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C146" s="14">
+        <v>2289120</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="15">
+        <v>41820</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" s="14">
+        <v>10504274</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="15">
+        <v>41820</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="14">
+        <v>2439968</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="15">
+        <v>41820</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C149" s="14">
+        <v>2273703</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="15">
+        <v>41820</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C150" s="14">
+        <v>1441486</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="15">
+        <v>41820</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C151" s="14">
+        <v>1123579</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B137" r:id="rId1" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B138" r:id="rId2" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B139" r:id="rId3" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B140" r:id="rId4" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B141" r:id="rId5" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B2" r:id="rId6" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B3" r:id="rId7" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B4" r:id="rId8" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B5" r:id="rId9" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B6" r:id="rId10" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B7" r:id="rId11" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B8" r:id="rId12" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B9" r:id="rId13" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B10" r:id="rId14" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B11" r:id="rId15" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B12" r:id="rId16" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B13" r:id="rId17" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B14" r:id="rId18" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B15" r:id="rId19" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B16" r:id="rId20" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B17" r:id="rId21" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B18" r:id="rId22" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B19" r:id="rId23" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B20" r:id="rId24" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B21" r:id="rId25" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B22" r:id="rId26" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B23" r:id="rId27" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B24" r:id="rId28" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B25" r:id="rId29" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B26" r:id="rId30" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B27" r:id="rId31" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B28" r:id="rId32" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B29" r:id="rId33" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B30" r:id="rId34" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B31" r:id="rId35" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B32" r:id="rId36" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B33" r:id="rId37" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B34" r:id="rId38" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B35" r:id="rId39" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B36" r:id="rId40" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B37" r:id="rId41" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B38" r:id="rId42" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B39" r:id="rId43" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B40" r:id="rId44" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B41" r:id="rId45" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B42" r:id="rId46" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B43" r:id="rId47" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B44" r:id="rId48" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B45" r:id="rId49" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B46" r:id="rId50" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B47" r:id="rId51" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B48" r:id="rId52" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B49" r:id="rId53" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B50" r:id="rId54" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B51" r:id="rId55" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B52" r:id="rId56" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B53" r:id="rId57" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B54" r:id="rId58" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B55" r:id="rId59" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B56" r:id="rId60" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B57" r:id="rId61" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B58" r:id="rId62" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B59" r:id="rId63" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B60" r:id="rId64" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B61" r:id="rId65" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B62" r:id="rId66" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B63" r:id="rId67" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B64" r:id="rId68" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B65" r:id="rId69" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B66" r:id="rId70" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B67" r:id="rId71" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B68" r:id="rId72" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B69" r:id="rId73" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B70" r:id="rId74" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B71" r:id="rId75" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B72" r:id="rId76" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B73" r:id="rId77" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B74" r:id="rId78" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B75" r:id="rId79" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B76" r:id="rId80" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B77" r:id="rId81" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B78" r:id="rId82" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B79" r:id="rId83" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B80" r:id="rId84" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B81" r:id="rId85" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B82" r:id="rId86" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B83" r:id="rId87" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B84" r:id="rId88" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B85" r:id="rId89" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B86" r:id="rId90" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B87" r:id="rId91" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B88" r:id="rId92" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B89" r:id="rId93" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B90" r:id="rId94" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B91" r:id="rId95" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B92" r:id="rId96" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B93" r:id="rId97" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B94" r:id="rId98" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B95" r:id="rId99" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B96" r:id="rId100" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B97" r:id="rId101" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B98" r:id="rId102" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B99" r:id="rId103" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B100" r:id="rId104" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B101" r:id="rId105" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B102" r:id="rId106" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B103" r:id="rId107" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B104" r:id="rId108" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B105" r:id="rId109" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B106" r:id="rId110" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B107" r:id="rId111" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B108" r:id="rId112" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B109" r:id="rId113" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B110" r:id="rId114" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B111" r:id="rId115" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B112" r:id="rId116" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B113" r:id="rId117" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B114" r:id="rId118" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B115" r:id="rId119" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B116" r:id="rId120" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B117" r:id="rId121" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B118" r:id="rId122" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B119" r:id="rId123" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B120" r:id="rId124" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B121" r:id="rId125" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B122" r:id="rId126" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B123" r:id="rId127" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B124" r:id="rId128" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B125" r:id="rId129" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B126" r:id="rId130" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B127" r:id="rId131" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B128" r:id="rId132" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B129" r:id="rId133" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B130" r:id="rId134" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B131" r:id="rId135" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B132" r:id="rId136" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B133" r:id="rId137" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B134" r:id="rId138" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B135" r:id="rId139" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B136" r:id="rId140" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B142" r:id="rId141" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B143" r:id="rId142" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B144" r:id="rId143" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B145" r:id="rId144" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B146" r:id="rId145" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B147" r:id="rId146" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B148" r:id="rId147" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B149" r:id="rId148" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B150" r:id="rId149" location="tab=summary#tab=box-office"/>
+    <hyperlink ref="B151" r:id="rId150" location="tab=summary#tab=box-office"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>